<commit_message>
i2c pretty much finished
</commit_message>
<xml_diff>
--- a/SN7 i2c & pins.xlsx
+++ b/SN7 i2c & pins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\targetarchitecture\esp32-rainbow-sparkle-unicorn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0D27AF-8E25-4EFD-8E67-F8AFC21A674F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81020C5F-4987-411F-A7E0-9A0EEC7EAF01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MQTT topics" sheetId="1" state="hidden" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="449">
   <si>
     <t>Action</t>
   </si>
@@ -1379,6 +1379,15 @@
   <si>
     <t>Switch interupt</t>
   </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>Pin state</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
 </sst>
 </file>
 
@@ -30175,7 +30184,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D5" sqref="B5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
@@ -30835,10 +30844,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1F20C5-E431-4F51-B98A-61CA1E4D1DB8}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
@@ -30982,23 +30991,19 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="33" t="s">
-        <v>268</v>
+        <v>87</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>312</v>
-      </c>
-      <c r="C7" s="49" t="s">
-        <v>399</v>
+        <v>446</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>400</v>
-      </c>
-      <c r="E7" s="50"/>
+        <v>447</v>
+      </c>
       <c r="F7" s="33" t="s">
-        <v>269</v>
-      </c>
-      <c r="G7" s="43" t="s">
-        <v>365</v>
+        <v>294</v>
+      </c>
+      <c r="G7" s="51" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
@@ -31006,7 +31011,7 @@
         <v>268</v>
       </c>
       <c r="B8" s="43" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C8" s="49" t="s">
         <v>399</v>
@@ -31016,7 +31021,7 @@
       </c>
       <c r="E8" s="50"/>
       <c r="F8" s="33" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G8" s="43" t="s">
         <v>365</v>
@@ -31024,20 +31029,20 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="33" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B9" s="43" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>272</v>
+        <v>399</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>275</v>
-      </c>
-      <c r="E9" s="33"/>
+        <v>400</v>
+      </c>
+      <c r="E9" s="50"/>
       <c r="F9" s="33" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="G9" s="43" t="s">
         <v>365</v>
@@ -31048,7 +31053,7 @@
         <v>271</v>
       </c>
       <c r="B10" s="43" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C10" s="49" t="s">
         <v>272</v>
@@ -31058,7 +31063,7 @@
       </c>
       <c r="E10" s="33"/>
       <c r="F10" s="33" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G10" s="43" t="s">
         <v>365</v>
@@ -31066,20 +31071,20 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="33" t="s">
-        <v>98</v>
+        <v>271</v>
       </c>
       <c r="B11" s="43" t="s">
-        <v>316</v>
-      </c>
-      <c r="C11" s="47" t="s">
-        <v>261</v>
+        <v>315</v>
+      </c>
+      <c r="C11" s="49" t="s">
+        <v>272</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
       <c r="E11" s="33"/>
-      <c r="F11" s="56" t="s">
-        <v>276</v>
+      <c r="F11" s="33" t="s">
+        <v>274</v>
       </c>
       <c r="G11" s="43" t="s">
         <v>365</v>
@@ -31090,7 +31095,7 @@
         <v>98</v>
       </c>
       <c r="B12" s="43" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C12" s="47" t="s">
         <v>261</v>
@@ -31100,7 +31105,7 @@
       </c>
       <c r="E12" s="33"/>
       <c r="F12" s="56" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G12" s="43" t="s">
         <v>365</v>
@@ -31111,7 +31116,7 @@
         <v>98</v>
       </c>
       <c r="B13" s="43" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C13" s="47" t="s">
         <v>261</v>
@@ -31121,7 +31126,7 @@
       </c>
       <c r="E13" s="33"/>
       <c r="F13" s="56" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G13" s="43" t="s">
         <v>365</v>
@@ -31132,7 +31137,7 @@
         <v>98</v>
       </c>
       <c r="B14" s="43" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C14" s="47" t="s">
         <v>261</v>
@@ -31142,7 +31147,7 @@
       </c>
       <c r="E14" s="33"/>
       <c r="F14" s="56" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G14" s="43" t="s">
         <v>365</v>
@@ -31153,7 +31158,7 @@
         <v>98</v>
       </c>
       <c r="B15" s="43" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C15" s="47" t="s">
         <v>261</v>
@@ -31163,7 +31168,7 @@
       </c>
       <c r="E15" s="33"/>
       <c r="F15" s="56" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G15" s="43" t="s">
         <v>365</v>
@@ -31174,7 +31179,7 @@
         <v>98</v>
       </c>
       <c r="B16" s="43" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C16" s="47" t="s">
         <v>261</v>
@@ -31184,7 +31189,7 @@
       </c>
       <c r="E16" s="33"/>
       <c r="F16" s="56" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G16" s="43" t="s">
         <v>365</v>
@@ -31195,7 +31200,7 @@
         <v>98</v>
       </c>
       <c r="B17" s="43" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C17" s="47" t="s">
         <v>261</v>
@@ -31205,7 +31210,7 @@
       </c>
       <c r="E17" s="33"/>
       <c r="F17" s="56" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G17" s="43" t="s">
         <v>365</v>
@@ -31216,7 +31221,7 @@
         <v>98</v>
       </c>
       <c r="B18" s="43" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C18" s="47" t="s">
         <v>261</v>
@@ -31226,7 +31231,7 @@
       </c>
       <c r="E18" s="33"/>
       <c r="F18" s="56" t="s">
-        <v>306</v>
+        <v>282</v>
       </c>
       <c r="G18" s="43" t="s">
         <v>365</v>
@@ -31237,7 +31242,7 @@
         <v>98</v>
       </c>
       <c r="B19" s="43" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C19" s="47" t="s">
         <v>261</v>
@@ -31247,7 +31252,7 @@
       </c>
       <c r="E19" s="33"/>
       <c r="F19" s="56" t="s">
-        <v>283</v>
+        <v>306</v>
       </c>
       <c r="G19" s="43" t="s">
         <v>365</v>
@@ -31258,7 +31263,7 @@
         <v>98</v>
       </c>
       <c r="B20" s="43" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C20" s="47" t="s">
         <v>261</v>
@@ -31268,7 +31273,7 @@
       </c>
       <c r="E20" s="33"/>
       <c r="F20" s="56" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G20" s="43" t="s">
         <v>365</v>
@@ -31279,7 +31284,7 @@
         <v>98</v>
       </c>
       <c r="B21" s="43" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C21" s="47" t="s">
         <v>261</v>
@@ -31289,7 +31294,7 @@
       </c>
       <c r="E21" s="33"/>
       <c r="F21" s="56" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G21" s="43" t="s">
         <v>365</v>
@@ -31300,7 +31305,7 @@
         <v>98</v>
       </c>
       <c r="B22" s="43" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C22" s="47" t="s">
         <v>261</v>
@@ -31310,7 +31315,7 @@
       </c>
       <c r="E22" s="33"/>
       <c r="F22" s="56" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G22" s="43" t="s">
         <v>365</v>
@@ -31321,7 +31326,7 @@
         <v>98</v>
       </c>
       <c r="B23" s="43" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C23" s="47" t="s">
         <v>261</v>
@@ -31331,7 +31336,7 @@
       </c>
       <c r="E23" s="33"/>
       <c r="F23" s="56" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G23" s="43" t="s">
         <v>365</v>
@@ -31342,7 +31347,7 @@
         <v>98</v>
       </c>
       <c r="B24" s="43" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C24" s="47" t="s">
         <v>261</v>
@@ -31352,7 +31357,7 @@
       </c>
       <c r="E24" s="33"/>
       <c r="F24" s="56" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G24" s="43" t="s">
         <v>365</v>
@@ -31363,7 +31368,7 @@
         <v>98</v>
       </c>
       <c r="B25" s="43" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C25" s="47" t="s">
         <v>261</v>
@@ -31373,48 +31378,52 @@
       </c>
       <c r="E25" s="33"/>
       <c r="F25" s="56" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G25" s="43" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="56" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="B26" s="57" t="s">
+      <c r="B26" s="43" t="s">
+        <v>330</v>
+      </c>
+      <c r="C26" s="47" t="s">
+        <v>261</v>
+      </c>
+      <c r="D26" s="33" t="s">
+        <v>291</v>
+      </c>
+      <c r="E26" s="33"/>
+      <c r="F26" s="56" t="s">
+        <v>289</v>
+      </c>
+      <c r="G26" s="43" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="56" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="57" t="s">
         <v>437</v>
       </c>
-      <c r="C26" s="58" t="s">
+      <c r="C27" s="58" t="s">
         <v>261</v>
       </c>
-      <c r="D26" s="56" t="s">
+      <c r="D27" s="56" t="s">
         <v>291</v>
       </c>
-      <c r="E26" s="56"/>
-      <c r="F26" s="56" t="s">
+      <c r="E27" s="56"/>
+      <c r="F27" s="56" t="s">
         <v>290</v>
       </c>
-      <c r="G26" s="57" t="s">
+      <c r="G27" s="57" t="s">
         <v>365</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A27" s="33" t="s">
-        <v>371</v>
-      </c>
-      <c r="B27" s="43" t="s">
-        <v>383</v>
-      </c>
-      <c r="C27" s="51" t="s">
-        <v>384</v>
-      </c>
-      <c r="D27" s="33" t="s">
-        <v>385</v>
-      </c>
-      <c r="F27" s="33" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
@@ -31422,13 +31431,13 @@
         <v>371</v>
       </c>
       <c r="B28" s="43" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="C28" s="51" t="s">
         <v>384</v>
       </c>
       <c r="D28" s="33" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="F28" s="33" t="s">
         <v>386</v>
@@ -31436,19 +31445,19 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="33" t="s">
-        <v>433</v>
+        <v>371</v>
       </c>
       <c r="B29" s="43" t="s">
-        <v>435</v>
+        <v>387</v>
       </c>
       <c r="C29" s="51" t="s">
-        <v>210</v>
+        <v>384</v>
       </c>
       <c r="D29" s="33" t="s">
-        <v>436</v>
+        <v>388</v>
       </c>
       <c r="F29" s="33" t="s">
-        <v>410</v>
+        <v>386</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
@@ -31456,26 +31465,43 @@
         <v>433</v>
       </c>
       <c r="B30" s="43" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="C30" s="51" t="s">
-        <v>261</v>
+        <v>210</v>
       </c>
       <c r="D30" s="33" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="F30" s="33" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A31" s="33"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="33"/>
-      <c r="F31" s="33"/>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D34" s="55"/>
+      <c r="A31" s="33" t="s">
+        <v>433</v>
+      </c>
+      <c r="B31" s="43" t="s">
+        <v>432</v>
+      </c>
+      <c r="C31" s="51" t="s">
+        <v>261</v>
+      </c>
+      <c r="D31" s="33" t="s">
+        <v>434</v>
+      </c>
+      <c r="F31" s="33" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A32" s="33"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="33"/>
+      <c r="F32" s="33"/>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D35" s="55"/>
     </row>
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>
@@ -37411,8 +37437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1006EC9-F903-45E1-9B2E-3BBE97776EFB}">
   <dimension ref="A1:F999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
removed the UART parsing method
</commit_message>
<xml_diff>
--- a/SN7 i2c & pins.xlsx
+++ b/SN7 i2c & pins.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\targetarchitecture\esp32-rainbow-sparkle-unicorn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B449C24-E53A-4DB3-93D5-CC12855463C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1DC03B-04AD-4D8D-90E2-1FB5804DEEA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MQTT topics" sheetId="1" state="hidden" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="449">
   <si>
     <t>Action</t>
   </si>
@@ -1381,16 +1381,13 @@
     <t>Check the flash times are the correct way around</t>
   </si>
   <si>
-    <t>Wifi SSID and password - need to allow spaces¬!</t>
-  </si>
-  <si>
-    <t>Connect EN pin to Microbit</t>
-  </si>
-  <si>
     <t>RESTART</t>
   </si>
   <si>
     <t>Resets the ESP32</t>
+  </si>
+  <si>
+    <t>add a reset method</t>
   </si>
 </sst>
 </file>
@@ -30188,10 +30185,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A7A2B5-CFDE-4DC2-BBB1-53E30A1E757A}">
-  <dimension ref="B2:B12"/>
+  <dimension ref="B2:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
@@ -30211,14 +30208,9 @@
         <v>445</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B8" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B12" t="s">
-        <v>447</v>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>448</v>
       </c>
     </row>
   </sheetData>
@@ -30230,7 +30222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784B3CAF-F768-478D-8F53-9C6BB6D54AC2}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -30843,10 +30835,10 @@
     <row r="35" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="33"/>
       <c r="B35" s="47" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D35" s="52" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E35" s="33"/>
     </row>

</xml_diff>

<commit_message>
added a reset method for the lighting
</commit_message>
<xml_diff>
--- a/SN7 i2c & pins.xlsx
+++ b/SN7 i2c & pins.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\targetarchitecture\esp32-rainbow-sparkle-unicorn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C296C43-0A5A-44AA-9C70-311890D71DAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FAF7ED-79B5-40B4-9215-DC6C3FC221D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="451">
   <si>
     <t>Action</t>
   </si>
@@ -1389,6 +1389,12 @@
   <si>
     <t>add a reset method</t>
   </si>
+  <si>
+    <t>Y4</t>
+  </si>
+  <si>
+    <t>Turns off all LEDs (resets controller)</t>
+  </si>
 </sst>
 </file>
 
@@ -30220,10 +30226,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784B3CAF-F768-478D-8F53-9C6BB6D54AC2}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
@@ -30486,30 +30492,26 @@
     </row>
     <row r="14" spans="1:7" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="33" t="s">
-        <v>166</v>
+        <v>105</v>
       </c>
       <c r="B14" s="43" t="s">
-        <v>351</v>
-      </c>
-      <c r="C14" s="51" t="s">
-        <v>353</v>
-      </c>
+        <v>449</v>
+      </c>
+      <c r="C14" s="51"/>
       <c r="D14" s="52" t="s">
-        <v>356</v>
+        <v>450</v>
       </c>
       <c r="E14" s="33" t="s">
-        <v>354</v>
-      </c>
-      <c r="F14" s="43" t="s">
-        <v>365</v>
-      </c>
+        <v>346</v>
+      </c>
+      <c r="F14" s="43"/>
     </row>
     <row r="15" spans="1:7" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="33" t="s">
         <v>166</v>
       </c>
       <c r="B15" s="43" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C15" s="51" t="s">
         <v>353</v>
@@ -30518,29 +30520,29 @@
         <v>356</v>
       </c>
       <c r="E15" s="33" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F15" s="43" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="34" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="34" t="s">
-        <v>271</v>
-      </c>
-      <c r="B16" s="54" t="s">
-        <v>359</v>
-      </c>
-      <c r="C16" s="54" t="s">
-        <v>360</v>
-      </c>
-      <c r="D16" s="34" t="s">
-        <v>362</v>
-      </c>
-      <c r="E16" s="34" t="s">
-        <v>273</v>
-      </c>
-      <c r="F16" s="54" t="s">
+    <row r="16" spans="1:7" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="B16" s="43" t="s">
+        <v>352</v>
+      </c>
+      <c r="C16" s="51" t="s">
+        <v>353</v>
+      </c>
+      <c r="D16" s="52" t="s">
+        <v>356</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>355</v>
+      </c>
+      <c r="F16" s="43" t="s">
         <v>365</v>
       </c>
     </row>
@@ -30549,36 +30551,39 @@
         <v>271</v>
       </c>
       <c r="B17" s="54" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C17" s="54" t="s">
         <v>360</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F17" s="54" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="33" t="s">
-        <v>371</v>
-      </c>
-      <c r="B18" s="43" t="s">
-        <v>372</v>
-      </c>
-      <c r="C18" s="51" t="s">
-        <v>373</v>
-      </c>
-      <c r="D18" s="52" t="s">
-        <v>374</v>
-      </c>
-      <c r="E18" s="33" t="s">
-        <v>375</v>
+    <row r="18" spans="1:6" s="34" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="34" t="s">
+        <v>271</v>
+      </c>
+      <c r="B18" s="54" t="s">
+        <v>361</v>
+      </c>
+      <c r="C18" s="54" t="s">
+        <v>360</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>363</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>274</v>
+      </c>
+      <c r="F18" s="54" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -30586,13 +30591,13 @@
         <v>371</v>
       </c>
       <c r="B19" s="43" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="D19" s="52" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="E19" s="33" t="s">
         <v>375</v>
@@ -30603,13 +30608,13 @@
         <v>371</v>
       </c>
       <c r="B20" s="43" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C20" s="51" t="s">
-        <v>428</v>
+        <v>382</v>
       </c>
       <c r="D20" s="52" t="s">
-        <v>429</v>
+        <v>380</v>
       </c>
       <c r="E20" s="33" t="s">
         <v>375</v>
@@ -30620,13 +30625,13 @@
         <v>371</v>
       </c>
       <c r="B21" s="43" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C21" s="51" t="s">
         <v>428</v>
       </c>
       <c r="D21" s="52" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E21" s="33" t="s">
         <v>375</v>
@@ -30637,13 +30642,13 @@
         <v>371</v>
       </c>
       <c r="B22" s="43" t="s">
-        <v>426</v>
+        <v>378</v>
       </c>
       <c r="C22" s="51" t="s">
         <v>428</v>
       </c>
       <c r="D22" s="52" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E22" s="33" t="s">
         <v>375</v>
@@ -30654,13 +30659,13 @@
         <v>371</v>
       </c>
       <c r="B23" s="43" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C23" s="51" t="s">
-        <v>381</v>
+        <v>428</v>
       </c>
       <c r="D23" s="52" t="s">
-        <v>379</v>
+        <v>431</v>
       </c>
       <c r="E23" s="33" t="s">
         <v>375</v>
@@ -30668,19 +30673,19 @@
     </row>
     <row r="24" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="33" t="s">
-        <v>151</v>
+        <v>371</v>
       </c>
       <c r="B24" s="43" t="s">
-        <v>401</v>
+        <v>427</v>
       </c>
       <c r="C24" s="51" t="s">
-        <v>360</v>
+        <v>381</v>
       </c>
       <c r="D24" s="52" t="s">
-        <v>402</v>
+        <v>379</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>269</v>
+        <v>375</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -30688,7 +30693,7 @@
         <v>151</v>
       </c>
       <c r="B25" s="43" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C25" s="51" t="s">
         <v>360</v>
@@ -30697,63 +30702,66 @@
         <v>402</v>
       </c>
       <c r="E25" s="33" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="33" t="s">
-        <v>404</v>
+        <v>151</v>
       </c>
       <c r="B26" s="43" t="s">
-        <v>405</v>
-      </c>
-      <c r="C26" s="47" t="s">
-        <v>411</v>
+        <v>403</v>
+      </c>
+      <c r="C26" s="51" t="s">
+        <v>360</v>
       </c>
       <c r="D26" s="52" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="E26" s="33" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="33" t="s">
         <v>404</v>
       </c>
       <c r="B27" s="43" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C27" s="47" t="s">
-        <v>412</v>
+        <v>411</v>
+      </c>
+      <c r="D27" s="52" t="s">
+        <v>407</v>
       </c>
       <c r="E27" s="33" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="33" t="s">
         <v>404</v>
       </c>
-      <c r="B28" s="47" t="s">
-        <v>413</v>
-      </c>
-      <c r="D28" s="34" t="s">
-        <v>414</v>
+      <c r="B28" s="43" t="s">
+        <v>406</v>
+      </c>
+      <c r="C28" s="47" t="s">
+        <v>412</v>
       </c>
       <c r="E28" s="33" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="33" t="s">
         <v>404</v>
       </c>
       <c r="B29" s="47" t="s">
-        <v>416</v>
-      </c>
-      <c r="C29" s="47" t="s">
-        <v>415</v>
+        <v>413</v>
+      </c>
+      <c r="D29" s="34" t="s">
+        <v>414</v>
       </c>
       <c r="E29" s="33" t="s">
         <v>410</v>
@@ -30764,10 +30772,10 @@
         <v>404</v>
       </c>
       <c r="B30" s="47" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="C30" s="47" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E30" s="33" t="s">
         <v>410</v>
@@ -30778,10 +30786,10 @@
         <v>404</v>
       </c>
       <c r="B31" s="47" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C31" s="47" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E31" s="33" t="s">
         <v>410</v>
@@ -30792,10 +30800,10 @@
         <v>404</v>
       </c>
       <c r="B32" s="47" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C32" s="47" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E32" s="33" t="s">
         <v>410</v>
@@ -30806,46 +30814,54 @@
         <v>404</v>
       </c>
       <c r="B33" s="47" t="s">
-        <v>424</v>
-      </c>
-      <c r="D33" s="33" t="s">
-        <v>420</v>
+        <v>423</v>
+      </c>
+      <c r="C33" s="47" t="s">
+        <v>419</v>
       </c>
       <c r="E33" s="33" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" s="33" t="s">
         <v>404</v>
       </c>
       <c r="B34" s="47" t="s">
-        <v>425</v>
-      </c>
-      <c r="C34" s="43" t="s">
-        <v>409</v>
-      </c>
-      <c r="D34" s="52" t="s">
-        <v>408</v>
+        <v>424</v>
+      </c>
+      <c r="D34" s="33" t="s">
+        <v>420</v>
       </c>
       <c r="E34" s="33" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="33"/>
+      <c r="A35" s="33" t="s">
+        <v>404</v>
+      </c>
       <c r="B35" s="47" t="s">
-        <v>446</v>
+        <v>425</v>
+      </c>
+      <c r="C35" s="43" t="s">
+        <v>409</v>
       </c>
       <c r="D35" s="52" t="s">
-        <v>447</v>
-      </c>
-      <c r="E35" s="33"/>
+        <v>408</v>
+      </c>
+      <c r="E35" s="33" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="36" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="33"/>
-      <c r="B36" s="47"/>
-      <c r="D36" s="52"/>
+      <c r="B36" s="47" t="s">
+        <v>446</v>
+      </c>
+      <c r="D36" s="52" t="s">
+        <v>447</v>
+      </c>
       <c r="E36" s="33"/>
     </row>
     <row r="37" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -30860,8 +30876,14 @@
       <c r="D38" s="52"/>
       <c r="E38" s="33"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D39" s="43"/>
+    <row r="39" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="33"/>
+      <c r="B39" s="47"/>
+      <c r="D39" s="52"/>
+      <c r="E39" s="33"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D40" s="43"/>
     </row>
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>

</xml_diff>

<commit_message>
touch is too sensitive
</commit_message>
<xml_diff>
--- a/SN7 i2c & pins.xlsx
+++ b/SN7 i2c & pins.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\targetarchitecture\esp32-rainbow-sparkle-unicorn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0165FBD0-43D8-4ECF-AC20-9B57C2B0F6A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8314BE-D28E-4923-8AE0-B04621011DD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="445">
   <si>
     <t>Action</t>
   </si>
@@ -835,9 +835,6 @@
     <t>Value(s)</t>
   </si>
   <si>
-    <t>1-12</t>
-  </si>
-  <si>
     <t>Pin touched</t>
   </si>
   <si>
@@ -1356,6 +1353,30 @@
   <si>
     <t>Expert</t>
   </si>
+  <si>
+    <t>0-11</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>ESP32</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>0-50</t>
+  </si>
+  <si>
+    <t>bounce delay</t>
+  </si>
+  <si>
+    <t>0-255,0-255</t>
+  </si>
+  <si>
+    <t>touchThreshold, releaseThreshold (must be lower than touch)</t>
+  </si>
 </sst>
 </file>
 
@@ -1590,7 +1611,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1686,6 +1707,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -30164,17 +30188,17 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -30186,16 +30210,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784B3CAF-F768-478D-8F53-9C6BB6D54AC2}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17.37890625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.234375" style="43" customWidth="1"/>
-    <col min="3" max="3" width="46.234375" style="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49" customWidth="1"/>
+    <col min="3" max="3" width="33.76171875" style="43" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.1875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.6171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -30213,10 +30237,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="46" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F1" s="46" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G1" s="46" t="s">
         <v>2</v>
@@ -30227,19 +30251,19 @@
         <v>8</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C2" s="49" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F2" s="47" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -30247,17 +30271,17 @@
         <v>8</v>
       </c>
       <c r="B3" s="43" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C3" s="48"/>
       <c r="D3" s="33" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F3" s="47" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
@@ -30265,17 +30289,17 @@
         <v>8</v>
       </c>
       <c r="B4" s="43" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C4" s="48"/>
       <c r="D4" s="33" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F4" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
@@ -30283,19 +30307,19 @@
         <v>8</v>
       </c>
       <c r="B5" s="43" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C5" s="49" t="s">
+        <v>280</v>
+      </c>
+      <c r="D5" s="33" t="s">
         <v>281</v>
       </c>
-      <c r="D5" s="33" t="s">
-        <v>282</v>
-      </c>
       <c r="E5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F5" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
@@ -30303,17 +30327,17 @@
         <v>8</v>
       </c>
       <c r="B6" s="43" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C6" s="49"/>
       <c r="D6" s="33" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F6" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
@@ -30321,17 +30345,17 @@
         <v>8</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C7" s="49"/>
       <c r="D7" s="33" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F7" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
@@ -30339,17 +30363,17 @@
         <v>8</v>
       </c>
       <c r="B8" s="43" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C8" s="49"/>
       <c r="D8" s="33" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F8" s="47" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
@@ -30357,17 +30381,17 @@
         <v>8</v>
       </c>
       <c r="B9" s="43" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C9" s="49"/>
       <c r="D9" s="33" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F9" s="47" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
@@ -30375,17 +30399,17 @@
         <v>8</v>
       </c>
       <c r="B10" s="43" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C10" s="47"/>
       <c r="D10" s="33" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F10" s="47" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -30393,19 +30417,19 @@
         <v>105</v>
       </c>
       <c r="B11" s="43" t="s">
+        <v>308</v>
+      </c>
+      <c r="C11" s="49" t="s">
         <v>309</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="D11" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>311</v>
-      </c>
       <c r="E11" s="33" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F11" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -30413,19 +30437,19 @@
         <v>105</v>
       </c>
       <c r="B12" s="43" t="s">
+        <v>311</v>
+      </c>
+      <c r="C12" s="51" t="s">
+        <v>316</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="C12" s="51" t="s">
-        <v>317</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>313</v>
-      </c>
       <c r="E12" s="33" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F12" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -30433,19 +30457,19 @@
         <v>105</v>
       </c>
       <c r="B13" s="43" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C13" s="51" t="s">
+        <v>317</v>
+      </c>
+      <c r="D13" s="52" t="s">
         <v>318</v>
       </c>
-      <c r="D13" s="52" t="s">
-        <v>319</v>
-      </c>
       <c r="E13" s="33" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F13" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -30453,14 +30477,14 @@
         <v>105</v>
       </c>
       <c r="B14" s="43" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C14" s="51"/>
       <c r="D14" s="52" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E14" s="33" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F14" s="43"/>
     </row>
@@ -30469,14 +30493,14 @@
         <v>105</v>
       </c>
       <c r="B15" s="43" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C15" s="51"/>
       <c r="D15" s="52" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E15" s="33" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F15" s="43"/>
     </row>
@@ -30485,19 +30509,19 @@
         <v>166</v>
       </c>
       <c r="B16" s="43" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C16" s="51" t="s">
+        <v>321</v>
+      </c>
+      <c r="D16" s="52" t="s">
+        <v>324</v>
+      </c>
+      <c r="E16" s="33" t="s">
         <v>322</v>
       </c>
-      <c r="D16" s="52" t="s">
-        <v>325</v>
-      </c>
-      <c r="E16" s="33" t="s">
-        <v>323</v>
-      </c>
       <c r="F16" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -30505,161 +30529,161 @@
         <v>166</v>
       </c>
       <c r="B17" s="43" t="s">
+        <v>320</v>
+      </c>
+      <c r="C17" s="51" t="s">
         <v>321</v>
       </c>
-      <c r="C17" s="51" t="s">
-        <v>322</v>
-      </c>
       <c r="D17" s="52" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E17" s="33" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F17" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="34" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="34" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B18" s="54" t="s">
+        <v>327</v>
+      </c>
+      <c r="C18" s="54" t="s">
         <v>328</v>
       </c>
-      <c r="C18" s="54" t="s">
-        <v>329</v>
-      </c>
       <c r="D18" s="34" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F18" s="54" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="34" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="34" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B19" s="54" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C19" s="54" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E19" s="34" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F19" s="54" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="33" t="s">
+        <v>339</v>
+      </c>
+      <c r="B20" s="43" t="s">
         <v>340</v>
       </c>
-      <c r="B20" s="43" t="s">
+      <c r="C20" s="51" t="s">
         <v>341</v>
       </c>
-      <c r="C20" s="51" t="s">
+      <c r="D20" s="52" t="s">
         <v>342</v>
       </c>
-      <c r="D20" s="52" t="s">
+      <c r="E20" s="33" t="s">
         <v>343</v>
-      </c>
-      <c r="E20" s="33" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="33" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B21" s="43" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C21" s="51" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D21" s="52" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E21" s="33" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="55" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="59" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B22" s="60" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C22" s="61" t="s">
+        <v>394</v>
+      </c>
+      <c r="D22" s="62" t="s">
         <v>395</v>
       </c>
-      <c r="D22" s="62" t="s">
-        <v>396</v>
-      </c>
       <c r="E22" s="59" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="55" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="59" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B23" s="60" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C23" s="61" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D23" s="62" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E23" s="59" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="33" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B24" s="43" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C24" s="51" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D24" s="52" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="33" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B25" s="43" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C25" s="51" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D25" s="52" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E25" s="33" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -30667,16 +30691,16 @@
         <v>151</v>
       </c>
       <c r="B26" s="43" t="s">
+        <v>367</v>
+      </c>
+      <c r="C26" s="51" t="s">
+        <v>328</v>
+      </c>
+      <c r="D26" s="52" t="s">
         <v>368</v>
       </c>
-      <c r="C26" s="51" t="s">
-        <v>329</v>
-      </c>
-      <c r="D26" s="52" t="s">
-        <v>369</v>
-      </c>
       <c r="E26" s="33" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -30684,224 +30708,249 @@
         <v>151</v>
       </c>
       <c r="B27" s="43" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C27" s="51" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D27" s="52" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E27" s="33" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="57" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="57" t="s">
+        <v>370</v>
+      </c>
+      <c r="B28" s="58" t="s">
         <v>371</v>
       </c>
-      <c r="B28" s="58" t="s">
-        <v>372</v>
-      </c>
       <c r="C28" s="58" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D28" s="57" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E28" s="57" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="57" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="57" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B29" s="58" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C29" s="58" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E29" s="57" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="33" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B30" s="47" t="s">
+        <v>379</v>
+      </c>
+      <c r="C30" s="43" t="s">
+        <v>426</v>
+      </c>
+      <c r="D30" s="34" t="s">
         <v>380</v>
       </c>
-      <c r="C30" s="43" t="s">
-        <v>427</v>
-      </c>
-      <c r="D30" s="34" t="s">
-        <v>381</v>
-      </c>
       <c r="E30" s="33" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="33" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B31" s="47" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C31" s="47" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E31" s="33" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="33" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B32" s="47" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C32" s="47" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E32" s="33" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" s="33" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B33" s="47" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C33" s="47" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E33" s="33" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" s="33" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B34" s="47" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C34" s="47" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E34" s="33" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35" s="33" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B35" s="47" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D35" s="33" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E35" s="33" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="33" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B36" s="47" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C36" s="43" t="s">
+        <v>375</v>
+      </c>
+      <c r="D36" s="52" t="s">
+        <v>374</v>
+      </c>
+      <c r="E36" s="33" t="s">
         <v>376</v>
-      </c>
-      <c r="D36" s="52" t="s">
-        <v>375</v>
-      </c>
-      <c r="E36" s="33" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="33" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B37" s="47" t="s">
+        <v>415</v>
+      </c>
+      <c r="C37" s="43" t="s">
         <v>416</v>
       </c>
-      <c r="C37" s="43" t="s">
+      <c r="D37" s="52" t="s">
         <v>417</v>
       </c>
-      <c r="D37" s="52" t="s">
-        <v>418</v>
-      </c>
       <c r="E37" s="33" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="33" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B38" s="47" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C38" s="43" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D38" s="52" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E38" s="33" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="33" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B39" s="47" t="s">
+        <v>422</v>
+      </c>
+      <c r="D39" s="52" t="s">
         <v>423</v>
       </c>
-      <c r="D39" s="52" t="s">
-        <v>424</v>
-      </c>
       <c r="E39" s="33" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="33" t="s">
-        <v>437</v>
+        <v>87</v>
       </c>
       <c r="B40" s="47" t="s">
+        <v>438</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="D40" s="52" t="s">
+        <v>444</v>
+      </c>
+      <c r="E40" s="33" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" s="47" t="s">
+        <v>440</v>
+      </c>
+      <c r="C41" s="63" t="s">
+        <v>441</v>
+      </c>
+      <c r="D41" s="52" t="s">
+        <v>442</v>
+      </c>
+      <c r="E41" s="33" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="33" t="s">
+        <v>436</v>
+      </c>
+      <c r="B42" s="47" t="s">
+        <v>411</v>
+      </c>
+      <c r="C42" s="52"/>
+      <c r="D42" s="52" t="s">
         <v>412</v>
       </c>
-      <c r="D40" s="52" t="s">
-        <v>413</v>
-      </c>
-      <c r="E40" s="33"/>
-    </row>
-    <row r="41" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="33"/>
-      <c r="B41" s="47"/>
-      <c r="D41" s="52"/>
-      <c r="E41" s="33"/>
-    </row>
-    <row r="42" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="33"/>
-      <c r="B42" s="47"/>
-      <c r="D42" s="52"/>
-      <c r="E42" s="33"/>
+      <c r="E42" s="33" t="s">
+        <v>439</v>
+      </c>
     </row>
     <row r="43" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="33"/>
@@ -30924,7 +30973,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
@@ -30955,10 +31004,10 @@
         <v>260</v>
       </c>
       <c r="F1" s="46" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G1" s="46" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
@@ -30966,7 +31015,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C2" s="47" t="s">
         <v>261</v>
@@ -30976,10 +31025,10 @@
       </c>
       <c r="E2" s="33"/>
       <c r="F2" s="33" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G2" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
@@ -30987,20 +31036,20 @@
         <v>8</v>
       </c>
       <c r="B3" s="43" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C3" s="51" t="s">
+        <v>275</v>
+      </c>
+      <c r="D3" s="33" t="s">
         <v>276</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>277</v>
       </c>
       <c r="E3" s="33"/>
       <c r="F3" s="33" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G3" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
@@ -31008,20 +31057,20 @@
         <v>8</v>
       </c>
       <c r="B4" s="43" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C4" s="49" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E4" s="50"/>
       <c r="F4" s="33" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G4" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
@@ -31029,20 +31078,20 @@
         <v>87</v>
       </c>
       <c r="B5" s="43" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C5" s="49" t="s">
+        <v>437</v>
+      </c>
+      <c r="D5" s="33" t="s">
         <v>264</v>
-      </c>
-      <c r="D5" s="33" t="s">
-        <v>265</v>
       </c>
       <c r="E5" s="50"/>
       <c r="F5" s="33" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G5" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
@@ -31050,104 +31099,104 @@
         <v>87</v>
       </c>
       <c r="B6" s="43" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C6" s="49" t="s">
-        <v>264</v>
+        <v>437</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E6" s="50"/>
       <c r="F6" s="33" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G6" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="33" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C7" s="49" t="s">
+        <v>365</v>
+      </c>
+      <c r="D7" s="33" t="s">
         <v>366</v>
-      </c>
-      <c r="D7" s="33" t="s">
-        <v>367</v>
       </c>
       <c r="E7" s="50"/>
       <c r="F7" s="33" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G7" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="33" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B8" s="43" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C8" s="49" t="s">
+        <v>365</v>
+      </c>
+      <c r="D8" s="33" t="s">
         <v>366</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>367</v>
       </c>
       <c r="E8" s="50"/>
       <c r="F8" s="33" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G8" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="B9" s="43" t="s">
+        <v>296</v>
+      </c>
+      <c r="C9" s="49" t="s">
         <v>271</v>
       </c>
-      <c r="B9" s="43" t="s">
-        <v>297</v>
-      </c>
-      <c r="C9" s="49" t="s">
-        <v>272</v>
-      </c>
       <c r="D9" s="33" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E9" s="50"/>
       <c r="F9" s="33" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G9" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>297</v>
+      </c>
+      <c r="C10" s="49" t="s">
         <v>271</v>
       </c>
-      <c r="B10" s="43" t="s">
-        <v>298</v>
-      </c>
-      <c r="C10" s="49" t="s">
-        <v>272</v>
-      </c>
       <c r="D10" s="33" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E10" s="50"/>
       <c r="F10" s="33" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G10" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="55" customFormat="1" x14ac:dyDescent="0.45">
@@ -31155,148 +31204,148 @@
         <v>98</v>
       </c>
       <c r="B11" s="43" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C11" s="49" t="s">
+        <v>429</v>
+      </c>
+      <c r="D11" s="33" t="s">
         <v>430</v>
-      </c>
-      <c r="D11" s="33" t="s">
-        <v>431</v>
       </c>
       <c r="E11" s="50"/>
       <c r="F11" s="33" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G11" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H11"/>
       <c r="I11"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="33" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B12" s="43" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C12" s="49" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E12" s="50"/>
       <c r="F12" s="33" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G12" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="33" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B13" s="43" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E13" s="50"/>
       <c r="F13" s="33" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G13" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="33" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B14" s="43" t="s">
+        <v>427</v>
+      </c>
+      <c r="C14" s="49" t="s">
+        <v>352</v>
+      </c>
+      <c r="D14" s="33" t="s">
         <v>428</v>
-      </c>
-      <c r="C14" s="49" t="s">
-        <v>353</v>
-      </c>
-      <c r="D14" s="33" t="s">
-        <v>429</v>
       </c>
       <c r="E14" s="50"/>
       <c r="F14" s="33" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G14" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="33" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B15" s="43" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C15" s="49" t="s">
         <v>210</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E15" s="50"/>
       <c r="F15" s="33" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G15" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="33" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B16" s="43" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C16" s="49" t="s">
         <v>261</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E16" s="50"/>
       <c r="F16" s="33" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G16" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="33" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B17" s="43" t="s">
+        <v>420</v>
+      </c>
+      <c r="C17" s="49" t="s">
+        <v>433</v>
+      </c>
+      <c r="D17" s="33" t="s">
         <v>421</v>
-      </c>
-      <c r="C17" s="49" t="s">
-        <v>434</v>
-      </c>
-      <c r="D17" s="33" t="s">
-        <v>422</v>
       </c>
       <c r="E17" s="50"/>
       <c r="F17" s="33" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G17" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
@@ -37255,7 +37304,7 @@
   <dimension ref="A1:F999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -37299,7 +37348,7 @@
     </row>
     <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="53" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B3" s="53" t="s">
         <v>35</v>
@@ -37313,7 +37362,7 @@
     </row>
     <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="53" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B4" s="53" t="s">
         <v>40</v>
@@ -37328,7 +37377,7 @@
     </row>
     <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="53" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B5" s="53" t="s">
         <v>55</v>
@@ -37343,7 +37392,7 @@
     </row>
     <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B6" s="53" t="s">
         <v>62</v>
@@ -37373,7 +37422,7 @@
     </row>
     <row r="8" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="53" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B8" s="53" t="s">
         <v>88</v>
@@ -37383,12 +37432,12 @@
         <v>90</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="53" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B9" s="53" t="s">
         <v>96</v>
@@ -37398,12 +37447,12 @@
         <v>97</v>
       </c>
       <c r="E9" s="53" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="53" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B10" s="53" t="s">
         <v>112</v>
@@ -37413,7 +37462,7 @@
         <v>114</v>
       </c>
       <c r="E10" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -37428,12 +37477,12 @@
         <v>126</v>
       </c>
       <c r="E11" s="53" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="53" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B12" s="53" t="s">
         <v>130</v>
@@ -37443,12 +37492,12 @@
         <v>131</v>
       </c>
       <c r="E12" s="53" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="53" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B13" s="53" t="s">
         <v>133</v>
@@ -37458,12 +37507,12 @@
         <v>134</v>
       </c>
       <c r="E13" s="53" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="53" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B14" s="53" t="s">
         <v>137</v>
@@ -37473,7 +37522,7 @@
         <v>138</v>
       </c>
       <c r="E14" s="53" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -41506,7 +41555,7 @@
     </row>
     <row r="2" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="53" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>21</v>
@@ -41578,7 +41627,7 @@
     </row>
     <row r="8" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="53" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>88</v>
@@ -41605,7 +41654,7 @@
         <v>114</v>
       </c>
       <c r="E10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -41617,7 +41666,7 @@
         <v>126</v>
       </c>
       <c r="E11" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -41629,7 +41678,7 @@
         <v>131</v>
       </c>
       <c r="E12" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -41641,7 +41690,7 @@
         <v>134</v>
       </c>
       <c r="E13" s="53" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
sorted a bug out in servo easing equation
</commit_message>
<xml_diff>
--- a/SN7 i2c & pins.xlsx
+++ b/SN7 i2c & pins.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\targetarchitecture\esp32-rainbow-sparkle-unicorn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8314BE-D28E-4923-8AE0-B04621011DD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5FCD17-08ED-4565-BC8E-AB702A8F5D33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MQTT topics" sheetId="1" state="hidden" r:id="rId1"/>
-    <sheet name="TODO" sheetId="9" r:id="rId2"/>
+    <sheet name="TODO" sheetId="9" state="hidden" r:id="rId2"/>
     <sheet name="Transmitted from Microbit" sheetId="6" r:id="rId3"/>
     <sheet name="Recieved on Microbit" sheetId="5" r:id="rId4"/>
     <sheet name="Actions" sheetId="2" state="hidden" r:id="rId5"/>
@@ -1225,9 +1225,6 @@
     <t>V6</t>
   </si>
   <si>
-    <t>0 - 15,0-180,0-180,20,minPulse,maxPulse</t>
-  </si>
-  <si>
     <t>ease servo between two angles (0-15) in a linear motion</t>
   </si>
   <si>
@@ -1376,6 +1373,9 @@
   </si>
   <si>
     <t>touchThreshold, releaseThreshold (must be lower than touch)</t>
+  </si>
+  <si>
+    <t>0 - 15,0-180,0-180,seconds,minPulse,maxPulse</t>
   </si>
 </sst>
 </file>
@@ -30181,24 +30181,24 @@
   <dimension ref="B2:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
   </sheetData>
@@ -30211,7 +30211,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
@@ -30477,11 +30477,11 @@
         <v>105</v>
       </c>
       <c r="B14" s="43" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C14" s="51"/>
       <c r="D14" s="52" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E14" s="33" t="s">
         <v>314</v>
@@ -30493,11 +30493,11 @@
         <v>105</v>
       </c>
       <c r="B15" s="43" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C15" s="51"/>
       <c r="D15" s="52" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E15" s="33" t="s">
         <v>314</v>
@@ -30626,10 +30626,10 @@
         <v>345</v>
       </c>
       <c r="C22" s="61" t="s">
+        <v>444</v>
+      </c>
+      <c r="D22" s="62" t="s">
         <v>394</v>
-      </c>
-      <c r="D22" s="62" t="s">
-        <v>395</v>
       </c>
       <c r="E22" s="59" t="s">
         <v>343</v>
@@ -30643,10 +30643,10 @@
         <v>346</v>
       </c>
       <c r="C23" s="61" t="s">
-        <v>394</v>
+        <v>444</v>
       </c>
       <c r="D23" s="62" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E23" s="59" t="s">
         <v>343</v>
@@ -30660,10 +30660,10 @@
         <v>392</v>
       </c>
       <c r="C24" s="51" t="s">
-        <v>394</v>
+        <v>444</v>
       </c>
       <c r="D24" s="52" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E24" s="33" t="s">
         <v>343</v>
@@ -30759,7 +30759,7 @@
         <v>379</v>
       </c>
       <c r="C30" s="43" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D30" s="34" t="s">
         <v>380</v>
@@ -30860,13 +30860,13 @@
         <v>370</v>
       </c>
       <c r="B37" s="47" t="s">
+        <v>414</v>
+      </c>
+      <c r="C37" s="43" t="s">
         <v>415</v>
       </c>
-      <c r="C37" s="43" t="s">
+      <c r="D37" s="52" t="s">
         <v>416</v>
-      </c>
-      <c r="D37" s="52" t="s">
-        <v>417</v>
       </c>
       <c r="E37" s="33" t="s">
         <v>376</v>
@@ -30877,13 +30877,13 @@
         <v>370</v>
       </c>
       <c r="B38" s="47" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C38" s="43" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D38" s="52" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E38" s="33" t="s">
         <v>376</v>
@@ -30894,10 +30894,10 @@
         <v>370</v>
       </c>
       <c r="B39" s="47" t="s">
+        <v>421</v>
+      </c>
+      <c r="D39" s="52" t="s">
         <v>422</v>
-      </c>
-      <c r="D39" s="52" t="s">
-        <v>423</v>
       </c>
       <c r="E39" s="33" t="s">
         <v>376</v>
@@ -30908,13 +30908,13 @@
         <v>87</v>
       </c>
       <c r="B40" s="47" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C40" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="D40" s="52" t="s">
         <v>443</v>
-      </c>
-      <c r="D40" s="52" t="s">
-        <v>444</v>
       </c>
       <c r="E40" s="33" t="s">
         <v>277</v>
@@ -30925,13 +30925,13 @@
         <v>87</v>
       </c>
       <c r="B41" s="47" t="s">
+        <v>439</v>
+      </c>
+      <c r="C41" s="63" t="s">
         <v>440</v>
       </c>
-      <c r="C41" s="63" t="s">
+      <c r="D41" s="52" t="s">
         <v>441</v>
-      </c>
-      <c r="D41" s="52" t="s">
-        <v>442</v>
       </c>
       <c r="E41" s="33" t="s">
         <v>277</v>
@@ -30939,17 +30939,17 @@
     </row>
     <row r="42" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="33" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B42" s="47" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C42" s="52"/>
       <c r="D42" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E42" s="33" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -31081,7 +31081,7 @@
         <v>292</v>
       </c>
       <c r="C5" s="49" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D5" s="33" t="s">
         <v>264</v>
@@ -31102,7 +31102,7 @@
         <v>293</v>
       </c>
       <c r="C6" s="49" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D6" s="33" t="s">
         <v>265</v>
@@ -31207,14 +31207,14 @@
         <v>298</v>
       </c>
       <c r="C11" s="49" t="s">
+        <v>428</v>
+      </c>
+      <c r="D11" s="33" t="s">
         <v>429</v>
-      </c>
-      <c r="D11" s="33" t="s">
-        <v>430</v>
       </c>
       <c r="E11" s="50"/>
       <c r="F11" s="33" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G11" s="43" t="s">
         <v>333</v>
@@ -31230,10 +31230,10 @@
         <v>351</v>
       </c>
       <c r="C12" s="49" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E12" s="50"/>
       <c r="F12" s="33" t="s">
@@ -31251,10 +31251,10 @@
         <v>354</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E13" s="50"/>
       <c r="F13" s="33" t="s">
@@ -31269,13 +31269,13 @@
         <v>339</v>
       </c>
       <c r="B14" s="43" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C14" s="49" t="s">
         <v>352</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E14" s="50"/>
       <c r="F14" s="33" t="s">
@@ -31287,16 +31287,16 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="33" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B15" s="43" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C15" s="49" t="s">
         <v>210</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E15" s="50"/>
       <c r="F15" s="33" t="s">
@@ -31308,16 +31308,16 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="33" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B16" s="43" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C16" s="49" t="s">
         <v>261</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E16" s="50"/>
       <c r="F16" s="33" t="s">
@@ -31329,16 +31329,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="33" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B17" s="43" t="s">
+        <v>419</v>
+      </c>
+      <c r="C17" s="49" t="s">
+        <v>432</v>
+      </c>
+      <c r="D17" s="33" t="s">
         <v>420</v>
-      </c>
-      <c r="C17" s="49" t="s">
-        <v>433</v>
-      </c>
-      <c r="D17" s="33" t="s">
-        <v>421</v>
       </c>
       <c r="E17" s="50"/>
       <c r="F17" s="33" t="s">
@@ -37348,7 +37348,7 @@
     </row>
     <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="53" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B3" s="53" t="s">
         <v>35</v>
@@ -37362,7 +37362,7 @@
     </row>
     <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="53" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B4" s="53" t="s">
         <v>40</v>
@@ -37377,7 +37377,7 @@
     </row>
     <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="53" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B5" s="53" t="s">
         <v>55</v>
@@ -37432,7 +37432,7 @@
         <v>90</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -37447,7 +37447,7 @@
         <v>97</v>
       </c>
       <c r="E9" s="53" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Added new method to obtain state of all switches
</commit_message>
<xml_diff>
--- a/SN7 i2c & pins.xlsx
+++ b/SN7 i2c & pins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\targetarchitecture\esp32-rainbow-sparkle-unicorn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5FCD17-08ED-4565-BC8E-AB702A8F5D33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5743F9BF-CB78-4319-BFC1-ACD39435AD83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MQTT topics" sheetId="1" state="hidden" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="451">
   <si>
     <t>Action</t>
   </si>
@@ -1377,6 +1377,24 @@
   <si>
     <t>0 - 15,0-180,0-180,seconds,minPulse,maxPulse</t>
   </si>
+  <si>
+    <t>0,1,1,1,2,1,3,1,4,1,5,1,6,1,7,1,8,1,9,1,10,1,11,1,12,1,13,1,14,1,15,0</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>returns button states</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>0,1,1,1,0,0</t>
+  </si>
+  <si>
+    <t>represent the digital state of all of the pins</t>
+  </si>
 </sst>
 </file>
 
@@ -30208,10 +30226,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784B3CAF-F768-478D-8F53-9C6BB6D54AC2}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
@@ -30937,29 +30955,44 @@
         <v>277</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="B42" s="43" t="s">
+        <v>448</v>
+      </c>
+      <c r="C42" s="49"/>
+      <c r="D42" s="33" t="s">
+        <v>447</v>
+      </c>
+      <c r="E42" s="33" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="33" t="s">
         <v>435</v>
       </c>
-      <c r="B42" s="47" t="s">
+      <c r="B43" s="47" t="s">
         <v>410</v>
       </c>
-      <c r="C42" s="52"/>
-      <c r="D42" s="52" t="s">
+      <c r="C43" s="52"/>
+      <c r="D43" s="52" t="s">
         <v>411</v>
       </c>
-      <c r="E42" s="33" t="s">
+      <c r="E43" s="33" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="33"/>
-      <c r="B43" s="47"/>
-      <c r="D43" s="52"/>
-      <c r="E43" s="33"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D44" s="43"/>
+    <row r="44" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="33"/>
+      <c r="B44" s="47"/>
+      <c r="D44" s="52"/>
+      <c r="E44" s="33"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D45" s="43"/>
     </row>
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>
@@ -30970,10 +31003,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1F20C5-E431-4F51-B98A-61CA1E4D1DB8}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
@@ -31222,39 +31255,39 @@
       <c r="H11"/>
       <c r="I11"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" s="55" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A12" s="33" t="s">
-        <v>339</v>
+        <v>98</v>
       </c>
       <c r="B12" s="43" t="s">
-        <v>351</v>
+        <v>446</v>
       </c>
       <c r="C12" s="49" t="s">
-        <v>431</v>
+        <v>449</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>433</v>
+        <v>450</v>
       </c>
       <c r="E12" s="50"/>
       <c r="F12" s="33" t="s">
-        <v>353</v>
-      </c>
-      <c r="G12" s="43" t="s">
-        <v>333</v>
-      </c>
+        <v>430</v>
+      </c>
+      <c r="G12" s="43"/>
+      <c r="H12"/>
+      <c r="I12"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="33" t="s">
         <v>339</v>
       </c>
       <c r="B13" s="43" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C13" s="49" t="s">
         <v>431</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E13" s="50"/>
       <c r="F13" s="33" t="s">
@@ -31269,13 +31302,13 @@
         <v>339</v>
       </c>
       <c r="B14" s="43" t="s">
-        <v>426</v>
+        <v>354</v>
       </c>
       <c r="C14" s="49" t="s">
-        <v>352</v>
+        <v>431</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>427</v>
+        <v>434</v>
       </c>
       <c r="E14" s="50"/>
       <c r="F14" s="33" t="s">
@@ -31287,20 +31320,20 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="33" t="s">
-        <v>398</v>
+        <v>339</v>
       </c>
       <c r="B15" s="43" t="s">
-        <v>400</v>
+        <v>426</v>
       </c>
       <c r="C15" s="49" t="s">
-        <v>210</v>
+        <v>352</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>401</v>
+        <v>427</v>
       </c>
       <c r="E15" s="50"/>
       <c r="F15" s="33" t="s">
-        <v>376</v>
+        <v>353</v>
       </c>
       <c r="G15" s="43" t="s">
         <v>333</v>
@@ -31311,13 +31344,13 @@
         <v>398</v>
       </c>
       <c r="B16" s="43" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="C16" s="49" t="s">
-        <v>261</v>
+        <v>210</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="E16" s="50"/>
       <c r="F16" s="33" t="s">
@@ -31332,13 +31365,13 @@
         <v>398</v>
       </c>
       <c r="B17" s="43" t="s">
-        <v>419</v>
+        <v>397</v>
       </c>
       <c r="C17" s="49" t="s">
-        <v>432</v>
+        <v>261</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>420</v>
+        <v>399</v>
       </c>
       <c r="E17" s="50"/>
       <c r="F17" s="33" t="s">
@@ -31349,11 +31382,25 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" s="33"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="33"/>
+      <c r="A18" s="33" t="s">
+        <v>398</v>
+      </c>
+      <c r="B18" s="43" t="s">
+        <v>419</v>
+      </c>
+      <c r="C18" s="49" t="s">
+        <v>432</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>420</v>
+      </c>
       <c r="E18" s="50"/>
-      <c r="F18" s="33"/>
+      <c r="F18" s="33" t="s">
+        <v>376</v>
+      </c>
+      <c r="G18" s="43" t="s">
+        <v>333</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="33"/>
@@ -31368,6 +31415,36 @@
       <c r="D20" s="33"/>
       <c r="E20" s="50"/>
       <c r="F20" s="33"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" s="33"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="33"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D26" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D28">
+        <f>LEN("0,0,0,0,0,0,0,0,0,0,0,0,0,0,0")</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D29">
+        <f>LEN("0,1,1,1,2,1,3,1,4,1,5,1,6,1,7,1,8,1,9,1,10,1,11,1,12,1,13,1,14,1,15,0")</f>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D31">
+        <f>69*8</f>
+        <v>552</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>

</xml_diff>

<commit_message>
clear down queue when STARTING command received on ESP32
</commit_message>
<xml_diff>
--- a/SN7 i2c & pins.xlsx
+++ b/SN7 i2c & pins.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\targetarchitecture\esp32-rainbow-sparkle-unicorn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5743F9BF-CB78-4319-BFC1-ACD39435AD83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B1D161-1AD8-4C97-B305-655855DBB78E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="452">
   <si>
     <t>Action</t>
   </si>
@@ -1378,9 +1378,6 @@
     <t>0 - 15,0-180,0-180,seconds,minPulse,maxPulse</t>
   </si>
   <si>
-    <t>0,1,1,1,2,1,3,1,4,1,5,1,6,1,7,1,8,1,9,1,10,1,11,1,12,1,13,1,14,1,15,0</t>
-  </si>
-  <si>
     <t>E2</t>
   </si>
   <si>
@@ -1394,6 +1391,12 @@
   </si>
   <si>
     <t>represent the digital state of all of the pins</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>Queue emptied</t>
   </si>
 </sst>
 </file>
@@ -30960,11 +30963,11 @@
         <v>98</v>
       </c>
       <c r="B42" s="43" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C42" s="49"/>
       <c r="D42" s="33" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E42" s="33" t="s">
         <v>430</v>
@@ -31003,10 +31006,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1F20C5-E431-4F51-B98A-61CA1E4D1DB8}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
@@ -31260,13 +31263,13 @@
         <v>98</v>
       </c>
       <c r="B12" s="43" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C12" s="49" t="s">
+        <v>448</v>
+      </c>
+      <c r="D12" s="33" t="s">
         <v>449</v>
-      </c>
-      <c r="D12" s="33" t="s">
-        <v>450</v>
       </c>
       <c r="E12" s="50"/>
       <c r="F12" s="33" t="s">
@@ -31403,11 +31406,20 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="33"/>
+      <c r="A19" s="33" t="s">
+        <v>435</v>
+      </c>
+      <c r="B19" s="43" t="s">
+        <v>450</v>
+      </c>
       <c r="C19" s="49"/>
-      <c r="D19" s="33"/>
+      <c r="D19" s="33" t="s">
+        <v>451</v>
+      </c>
       <c r="E19" s="50"/>
-      <c r="F19" s="33"/>
+      <c r="F19" s="33" t="s">
+        <v>438</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="33"/>
@@ -31422,29 +31434,6 @@
       <c r="D21" s="33"/>
       <c r="E21" s="50"/>
       <c r="F21" s="33"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="D26" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="D28">
-        <f>LEN("0,0,0,0,0,0,0,0,0,0,0,0,0,0,0")</f>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="D29">
-        <f>LEN("0,1,1,1,2,1,3,1,4,1,5,1,6,1,7,1,8,1,9,1,10,1,11,1,12,1,13,1,14,1,15,0")</f>
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="D31">
-        <f>69*8</f>
-        <v>552</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>

</xml_diff>

<commit_message>
Revert "Update SN7 i2c & pins.xlsx"
This reverts commit bd0644bf1be158c40aa0137e9429aabf76cfc7e4.
</commit_message>
<xml_diff>
--- a/SN7 i2c & pins.xlsx
+++ b/SN7 i2c & pins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\targetarchitecture\esp32-rainbow-sparkle-unicorn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B52985F-690E-489A-940C-6364F885CBDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B1D161-1AD8-4C97-B305-655855DBB78E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MQTT topics" sheetId="1" state="hidden" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="452">
   <si>
     <t>Action</t>
   </si>
@@ -1398,9 +1398,6 @@
   <si>
     <t>Queue emptied</t>
   </si>
-  <si>
-    <t>CLEARQ</t>
-  </si>
 </sst>
 </file>
 
@@ -30234,8 +30231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784B3CAF-F768-478D-8F53-9C6BB6D54AC2}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
@@ -30992,12 +30989,8 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="33" t="s">
-        <v>435</v>
-      </c>
-      <c r="B44" s="43" t="s">
-        <v>452</v>
-      </c>
+      <c r="A44" s="33"/>
+      <c r="B44" s="47"/>
       <c r="D44" s="52"/>
       <c r="E44" s="33"/>
     </row>
@@ -31015,8 +31008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1F20C5-E431-4F51-B98A-61CA1E4D1DB8}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>

</xml_diff>